<commit_message>
2D Images Interactor Changed
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Hours</t>
   </si>
@@ -91,13 +91,19 @@
   </si>
   <si>
     <t>• Test Tracker Python Code in Linux (Ubuntu)</t>
+  </si>
+  <si>
+    <t>• Python Tracker Connection (Aurora)</t>
+  </si>
+  <si>
+    <t>* OV Preparation &amp; Build</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,8 +173,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,8 +228,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -265,12 +282,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -338,6 +394,24 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -619,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G34"/>
+  <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +924,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -864,67 +938,83 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+      <c r="A27" s="32"/>
+      <c r="B27" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="34">
+        <v>5</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="2">
-        <v>8</v>
-      </c>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
+      <c r="C28" s="30">
+        <v>2</v>
       </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C29" s="2">
-        <v>3</v>
-      </c>
-      <c r="E29" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+      <c r="E30" s="24"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="s">
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="19">
-        <f>SUM(C27:C31)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="19">
+        <f>SUM(C27:C32)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D34" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="21">
         <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="21">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added slider to 2D viewports
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -685,7 +685,7 @@
   <dimension ref="A2:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,14 +1046,18 @@
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
       <c r="E40" s="11"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="2"/>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
       <c r="E41" s="11" t="s">
         <v>26</v>
       </c>
@@ -1076,7 +1080,7 @@
       </c>
       <c r="C44" s="19">
         <f>SUM(C39:C43)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1091,7 +1095,9 @@
       <c r="C46" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="21"/>
+      <c r="D46" s="21">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
set nd get cam props in 3D viewer
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Hours</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>شهریور 98</t>
+  </si>
+  <si>
+    <t>* BronchoVision Viewers</t>
   </si>
 </sst>
 </file>
@@ -682,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,39 +1067,35 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C42" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="2"/>
+      <c r="B43" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="19">
+        <f>SUM(C39:C42)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="19">
-        <f>SUM(C39:C43)</f>
-        <v>7</v>
+      <c r="C44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" s="21">
-        <v>4</v>
+      <c r="D45" s="21">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trajectory of points added
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t>Hours</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>مهر 98</t>
+  </si>
+  <si>
+    <t>• Read points from .mat file</t>
+  </si>
+  <si>
+    <t>• Draw trajectory of points in 3D</t>
   </si>
 </sst>
 </file>
@@ -701,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G55"/>
+  <dimension ref="A2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,59 +1151,59 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
-      <c r="B49" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" s="30"/>
-      <c r="E49" s="11"/>
+      <c r="B49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
       <c r="B50" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="E50" s="11"/>
+        <v>28</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="E51" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="C51" s="2">
+        <v>4</v>
+      </c>
+      <c r="E51" s="37"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52" s="2">
-        <v>3</v>
-      </c>
-      <c r="E52" s="37"/>
+      <c r="B52" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="19">
+        <f>SUM(C49:C51)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="19">
-        <f>SUM(C49:C52)</f>
+      <c r="C53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C54" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" s="21">
-        <v>0</v>
+      <c r="D54" s="21">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally! Virtual Cam worked
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>Hours</t>
   </si>
@@ -126,10 +126,13 @@
     <t>مهر 98</t>
   </si>
   <si>
-    <t>• Read points from .mat file</t>
-  </si>
-  <si>
     <t>• Draw trajectory of points in 3D</t>
+  </si>
+  <si>
+    <t>• 3D Virtual camera (on registered points)</t>
+  </si>
+  <si>
+    <t>• Read registered points from .mat file</t>
   </si>
 </sst>
 </file>
@@ -710,7 +713,7 @@
   <dimension ref="A2:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1169,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,9 +1180,11 @@
         <v>31</v>
       </c>
       <c r="C51" s="2">
-        <v>4</v>
-      </c>
-      <c r="E51" s="37"/>
+        <v>6</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="18" t="s">
@@ -1187,7 +1192,7 @@
       </c>
       <c r="C52" s="19">
         <f>SUM(C49:C51)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1203,7 +1208,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="21">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flip points instead of image
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="C50" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>37</v>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="C54" s="19">
         <f>SUM(C49:C53)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="21">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aded ResetVB and ResetViews
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>Hours</t>
   </si>
@@ -123,9 +123,6 @@
     <t>مهر 98</t>
   </si>
   <si>
-    <t>• 3D Virtual camera (on registered points)</t>
-  </si>
-  <si>
     <t>• Read registered points from .mat file</t>
   </si>
   <si>
@@ -142,6 +139,12 @@
   </si>
   <si>
     <t>• First Stable Release</t>
+  </si>
+  <si>
+    <t>• Update 2D views in VB mode</t>
+  </si>
+  <si>
+    <t>• 3D Virtual Bronchoscopy (on registered points)</t>
   </si>
 </sst>
 </file>
@@ -729,7 +732,7 @@
   <dimension ref="A2:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,7 +741,7 @@
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
@@ -1102,7 +1105,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="2">
         <v>4</v>
@@ -1183,18 +1186,18 @@
         <v>9</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="2">
+        <v>18</v>
+      </c>
+      <c r="E50" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="C50" s="2">
-        <v>14</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -1205,12 +1208,12 @@
         <v>6</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C52" s="2">
         <v>2</v>
@@ -1221,12 +1224,14 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C53" s="2">
         <v>1</v>
       </c>
-      <c r="E53" s="36"/>
+      <c r="E53" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="18" t="s">
@@ -1234,8 +1239,9 @@
       </c>
       <c r="C54" s="19">
         <f>SUM(C49:C53)</f>
-        <v>32</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E54" s="36"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C55" s="4" t="s">
@@ -1250,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="21">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2D slice sliders in VB
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -733,7 +733,7 @@
   <dimension ref="A2:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1202,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>33</v>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="C57" s="19">
         <f>SUM(C51:C56)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
         <v>3</v>
       </c>
       <c r="D59" s="21">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last Changes for better 3D surface
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t>Hours</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>* Data Importing</t>
+  </si>
+  <si>
+    <t>آبان 98</t>
+  </si>
+  <si>
+    <t>• Fill holes in 3D view</t>
   </si>
 </sst>
 </file>
@@ -724,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G59"/>
+  <dimension ref="A2:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:E59"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,14 +1176,14 @@
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="36"/>
       <c r="B49" s="36"/>
       <c r="C49" s="36"/>
       <c r="D49" s="36"/>
       <c r="E49" s="36"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>32</v>
       </c>
@@ -1191,7 +1197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>16</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>39</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1224,7 +1230,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>36</v>
       </c>
@@ -1235,7 +1241,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>41</v>
       </c>
@@ -1244,7 +1250,7 @@
       </c>
       <c r="E55" s="35"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>35</v>
       </c>
@@ -1253,7 +1259,7 @@
       </c>
       <c r="E56" s="35"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" s="18" t="s">
         <v>4</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C58" s="4" t="s">
         <v>2</v>
       </c>
@@ -1270,12 +1276,111 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C59" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D59" s="21">
         <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="36"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="36"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="E63" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="E64" s="11"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="2">
+        <v>2</v>
+      </c>
+      <c r="E65" s="11"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="E66" s="11"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="E67" s="35"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="E68" s="35"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="19">
+        <f>SUM(C63:C68)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pyinstaller spec file corrected
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -742,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G88"/>
+  <dimension ref="A2:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1525,7 @@
         <v>17</v>
       </c>
       <c r="C84" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E84" s="11"/>
     </row>
@@ -1538,28 +1538,32 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C86" s="19">
-        <f>SUM(C84:C84)</f>
-        <v>2</v>
-      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="2"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D87" s="3">
-        <v>2</v>
+      <c r="B87" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="19">
+        <f>SUM(C84:C86)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C88" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C89" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D88" s="21">
-        <v>2</v>
+      <c r="D89" s="21">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Show tool on views (unregistered)
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
   <si>
     <t>Hours</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>* Visualize Tool in Viewers</t>
+  </si>
+  <si>
+    <t>* Registration</t>
   </si>
 </sst>
 </file>
@@ -754,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G89"/>
+  <dimension ref="A2:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,12 +1472,8 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C77" s="2">
-        <v>0</v>
-      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="2"/>
       <c r="E77" s="11"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -1563,28 +1562,36 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C87" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="19">
-        <f>SUM(C84:C86)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D88" s="3">
-        <v>2</v>
+      <c r="C88" s="19">
+        <f>SUM(C84:C87)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C89" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C90" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D89" s="21">
-        <v>6</v>
+      <c r="D90" s="21">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GUI updates + fixed resetViewports to reset slider values
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1547,7 @@
         <v>47</v>
       </c>
       <c r="C85" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>50</v>
@@ -1558,7 +1558,7 @@
         <v>48</v>
       </c>
       <c r="C86" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -1566,7 +1566,7 @@
         <v>51</v>
       </c>
       <c r="C87" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="C88" s="19">
         <f>SUM(C84:C87)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="D89" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -1591,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="D90" s="21">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last stable for ine 3D and three 2D views
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
   <si>
     <t>Hours</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>* Registration</t>
+  </si>
+  <si>
+    <t>* Video Capture</t>
+  </si>
+  <si>
+    <t>* 2D/3D Views</t>
   </si>
 </sst>
 </file>
@@ -757,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G90"/>
+  <dimension ref="A2:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+      <selection activeCell="M96" sqref="M96:R96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,40 +1564,56 @@
         <v>48</v>
       </c>
       <c r="C86" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C88" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C88" s="19">
-        <f>SUM(C84:C87)</f>
-        <v>14</v>
-      </c>
-    </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="4" t="s">
+      <c r="B89" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="19">
+        <f>SUM(C84:C89)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C91" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D89" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="4" t="s">
+      <c r="D91" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C92" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D90" s="21">
-        <v>10</v>
+      <c r="D92" s="21">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new layout views are ready
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -766,7 +766,7 @@
   <dimension ref="A2:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="M96" sqref="M96:R96"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1572,7 @@
         <v>53</v>
       </c>
       <c r="C87" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="C90" s="19">
         <f>SUM(C84:C89)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="D92" s="21">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cross in 3D view
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -168,9 +168,6 @@
     <t>* Tracker DataCapture</t>
   </si>
   <si>
-    <t>* Get Tool/Ref Coordinates</t>
-  </si>
-  <si>
     <t>* Visualize Tool in Viewers</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>* 2D/3D Views</t>
+  </si>
+  <si>
+    <t>* Get Tool/Ref Coordinates from Tracker</t>
   </si>
 </sst>
 </file>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,7 +1352,7 @@
         <v>40</v>
       </c>
       <c r="C63" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" s="11" t="s">
         <v>43</v>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C64" s="19">
         <f>SUM(C63:C63)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -1380,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="D66" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1542,10 +1542,10 @@
         <v>17</v>
       </c>
       <c r="C84" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E84" s="39" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -1553,10 +1553,10 @@
         <v>47</v>
       </c>
       <c r="C85" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -1569,26 +1569,26 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C87" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C88" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C89" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="C90" s="19">
         <f>SUM(C84:C89)</f>
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="D91" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="D92" s="21">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Decimation is tested (commented)
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -766,7 +766,7 @@
   <dimension ref="A2:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,7 +1580,7 @@
         <v>50</v>
       </c>
       <c r="C88" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="C90" s="19">
         <f>SUM(C84:C89)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="D92" s="21">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
editable regMat window added
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>Hours</t>
   </si>
@@ -147,30 +147,9 @@
     <t>* Data Importing</t>
   </si>
   <si>
-    <t>آبان 98</t>
-  </si>
-  <si>
-    <t>• Fill holes in 3D view</t>
-  </si>
-  <si>
-    <t>آذر 98</t>
-  </si>
-  <si>
-    <t>دی 98</t>
-  </si>
-  <si>
-    <t>بهمن 98</t>
-  </si>
-  <si>
-    <t>* Tracker GUI</t>
-  </si>
-  <si>
     <t>* Tracker DataCapture</t>
   </si>
   <si>
-    <t>* Visualize Tool in Viewers</t>
-  </si>
-  <si>
     <t>* Registration</t>
   </si>
   <si>
@@ -181,6 +160,27 @@
   </si>
   <si>
     <t>* Get Tool/Ref Coordinates from Tracker</t>
+  </si>
+  <si>
+    <t>* CenterLine Extraction</t>
+  </si>
+  <si>
+    <t>* Visualize Tool in Viewers (2D/3D)</t>
+  </si>
+  <si>
+    <t>* GUI</t>
+  </si>
+  <si>
+    <t>* Virtual Camera</t>
+  </si>
+  <si>
+    <t>آبان تا بهمن 98</t>
+  </si>
+  <si>
+    <t>* Improved 3D Views</t>
+  </si>
+  <si>
+    <t>* Apply Registration</t>
   </si>
 </sst>
 </file>
@@ -763,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G92"/>
+  <dimension ref="A2:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>10</v>
@@ -1349,271 +1349,111 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C63" s="2">
+        <v>5</v>
+      </c>
+      <c r="E63" s="39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="2">
+        <v>6</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C65" s="2">
+        <v>5</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="2">
+        <v>7</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" s="2">
         <v>3</v>
       </c>
-      <c r="E63" s="11" t="s">
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="18" t="s">
+      <c r="C68" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="19">
-        <f>SUM(C63:C63)</f>
+      <c r="C72" s="19">
+        <f>SUM(C63:C71)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C74" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D66" s="21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="36"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C70" s="2">
-        <v>3</v>
-      </c>
-      <c r="E70" s="11"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C71" s="19">
-        <f>SUM(C70:C70)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D72" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D73" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="36"/>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76" s="23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-      <c r="C77" s="2"/>
-      <c r="E77" s="11"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78" s="19">
-        <f>SUM(C77:C77)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D79" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D80" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="14"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="36"/>
-      <c r="B82" s="36"/>
-      <c r="C82" s="36"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C84" s="2">
-        <v>5</v>
-      </c>
-      <c r="E84" s="39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C85" s="2">
-        <v>5</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C86" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C87" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C88" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C89" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C90" s="19">
-        <f>SUM(C84:C89)</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D91" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D92" s="21">
-        <v>23</v>
+      <c r="D74" s="21">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multithreading using threading module
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>Hours</t>
   </si>
@@ -171,16 +171,25 @@
     <t>* GUI</t>
   </si>
   <si>
-    <t>* Virtual Camera</t>
-  </si>
-  <si>
     <t>آبان تا بهمن 98</t>
   </si>
   <si>
     <t>* Improved 3D Views</t>
   </si>
   <si>
-    <t>* Apply Registration</t>
+    <t>* 3D Virtual View</t>
+  </si>
+  <si>
+    <t>* Live Tracking (Pre-registered)</t>
+  </si>
+  <si>
+    <t>اسفند 98</t>
+  </si>
+  <si>
+    <t>Multithreading</t>
+  </si>
+  <si>
+    <t>* Multithread Tracking</t>
   </si>
 </sst>
 </file>
@@ -763,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G74"/>
+  <dimension ref="A2:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,7 +1344,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>10</v>
@@ -1369,7 +1378,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>42</v>
       </c>
@@ -1377,10 +1386,10 @@
         <v>5</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>45</v>
       </c>
@@ -1391,15 +1400,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C67" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>43</v>
       </c>
@@ -1407,7 +1416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>47</v>
       </c>
@@ -1415,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>44</v>
       </c>
@@ -1423,7 +1432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>13</v>
       </c>
@@ -1431,7 +1440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" s="18" t="s">
         <v>4</v>
       </c>
@@ -1440,7 +1449,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C73" s="4" t="s">
         <v>2</v>
       </c>
@@ -1448,12 +1457,113 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C74" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="21">
         <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="36"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+      <c r="C79" s="2"/>
+      <c r="E79" s="11"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="1"/>
+      <c r="C80" s="2"/>
+      <c r="E80" s="11"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="1"/>
+      <c r="C81" s="2"/>
+      <c r="E81" s="11"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="1"/>
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="1"/>
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="1"/>
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="1"/>
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="19">
+        <f>SUM(C78:C86)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C88" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C89" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="21">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QVTKViewer parent class and 2D/3D inheritances
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>Hours</t>
   </si>
@@ -183,9 +183,6 @@
     <t>* Live Tracking (Pre-registered)</t>
   </si>
   <si>
-    <t>اسفند 98</t>
-  </si>
-  <si>
     <t>Multithreading</t>
   </si>
   <si>
@@ -193,6 +190,12 @@
   </si>
   <si>
     <t>Code Refactoring</t>
+  </si>
+  <si>
+    <t>اسفند 98 تا خرداد 99</t>
+  </si>
+  <si>
+    <t>Documents (Read/Write)</t>
   </si>
 </sst>
 </file>
@@ -777,13 +780,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
@@ -1346,7 +1349,7 @@
       <c r="E61" s="36"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="32" t="s">
         <v>50</v>
       </c>
       <c r="B62" s="7" t="s">
@@ -1444,10 +1447,10 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="19">
+      <c r="C72" s="34">
         <f>SUM(C63:C71)</f>
         <v>40</v>
       </c>
@@ -1486,7 +1489,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="25" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>10</v>
@@ -1500,27 +1503,31 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C79" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E79" s="11"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="1"/>
-      <c r="C80" s="2"/>
+      <c r="B80" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C80" s="2">
+        <v>3</v>
+      </c>
       <c r="E80" s="11"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
@@ -1554,7 +1561,7 @@
       </c>
       <c r="C87" s="19">
         <f>SUM(C78:C86)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
@@ -1570,7 +1577,7 @@
         <v>3</v>
       </c>
       <c r="D89" s="21">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>